<commit_message>
ready to plot distributions
</commit_message>
<xml_diff>
--- a/Project 2/data_sets/arrival_02.xlsx
+++ b/Project 2/data_sets/arrival_02.xlsx
@@ -58,7 +58,7 @@
     <t>11:58:26</t>
   </si>
   <si>
-    <t>12:00:34</t>
+    <t>12:01:34</t>
   </si>
   <si>
     <t>12:01:36</t>
@@ -536,7 +536,7 @@
     <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>